<commit_message>
update tests for named columns with missing data
</commit_message>
<xml_diff>
--- a/tests/testthat/empty-named-column.xlsx
+++ b/tests/testthat/empty-named-column.xlsx
@@ -369,46 +369,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="B1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>